<commit_message>
échange, jour et mois excel
</commit_message>
<xml_diff>
--- a/Liste des films 2025.xlsx
+++ b/Liste des films 2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcgks\OneDrive\Documentos\Cine2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{798E186F-477B-493A-B935-92BAEBE82796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C026B116-EFBC-4FCA-A1D9-2C0BF418FF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FF3FF06F-F152-4A1B-B3A0-020A35EDB07F}"/>
+    <workbookView xWindow="-19310" yWindow="-610" windowWidth="19420" windowHeight="10300" xr2:uid="{FF3FF06F-F152-4A1B-B3A0-020A35EDB07F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
   <si>
     <t>Janvier</t>
   </si>
@@ -290,8 +290,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65DD31D5-8922-4AD2-8A66-DF40B6A35778}" name="Tableau1" displayName="Tableau1" ref="A1:C47" totalsRowShown="0">
   <autoFilter ref="A1:C47" xr:uid="{65DD31D5-8922-4AD2-8A66-DF40B6A35778}"/>
   <tableColumns count="3">
+    <tableColumn id="2" xr3:uid="{7C060F9F-9CAF-4B38-BA77-A715BFF1FF94}" name="Jour" dataDxfId="0"/>
     <tableColumn id="1" xr3:uid="{1AE7041B-F879-49BD-9A5D-BE2569BDC666}" name="Mois"/>
-    <tableColumn id="2" xr3:uid="{64359F4E-CAB9-4217-837B-87E23B5B8AC0}" name="Jour" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{C85DC129-82D6-4530-AC26-8C93F095D4E1}" name="Titre"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -618,7 +618,7 @@
   <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -628,516 +628,516 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" t="s">
-        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>0</v>
-      </c>
-      <c r="B3" s="1">
-        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
         <v>0</v>
-      </c>
-      <c r="B4" s="1">
-        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
         <v>0</v>
-      </c>
-      <c r="B5" s="1">
-        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
-      </c>
-      <c r="B8" s="1">
-        <v>5</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>14</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
-      </c>
-      <c r="B10" s="1">
-        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
         <v>8</v>
-      </c>
-      <c r="B11" s="1">
-        <v>26</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
         <v>13</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="1">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
-      </c>
-      <c r="B13" s="1">
-        <v>16</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="1">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
         <v>13</v>
-      </c>
-      <c r="B14" s="1">
-        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="1">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
         <v>13</v>
-      </c>
-      <c r="B15" s="1">
-        <v>30</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
         <v>18</v>
-      </c>
-      <c r="B16" s="1">
-        <v>14</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="1">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
         <v>18</v>
-      </c>
-      <c r="B17" s="1">
-        <v>21</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="1">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
         <v>18</v>
-      </c>
-      <c r="B18" s="1">
-        <v>21</v>
       </c>
       <c r="C18" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="1">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
         <v>18</v>
-      </c>
-      <c r="B19" s="1">
-        <v>28</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="1">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
         <v>23</v>
-      </c>
-      <c r="B20" s="1">
-        <v>4</v>
       </c>
       <c r="C20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="1">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
         <v>23</v>
-      </c>
-      <c r="B21" s="1">
-        <v>11</v>
       </c>
       <c r="C21" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="1">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
         <v>23</v>
-      </c>
-      <c r="B22" s="1">
-        <v>18</v>
       </c>
       <c r="C22" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="1">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
         <v>23</v>
-      </c>
-      <c r="B23" s="1">
-        <v>18</v>
       </c>
       <c r="C23" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="1">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
         <v>23</v>
-      </c>
-      <c r="B24" s="1">
-        <v>25</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="1">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
         <v>23</v>
-      </c>
-      <c r="B25" s="1">
-        <v>25</v>
       </c>
       <c r="C25" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="1">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
         <v>30</v>
-      </c>
-      <c r="B26" s="1">
-        <v>4</v>
       </c>
       <c r="C26" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="1">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
         <v>32</v>
-      </c>
-      <c r="B27" s="1">
-        <v>9</v>
       </c>
       <c r="C27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="1">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
         <v>30</v>
-      </c>
-      <c r="B28" s="1">
-        <v>16</v>
       </c>
       <c r="C28" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="1">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
         <v>30</v>
-      </c>
-      <c r="B29" s="1">
-        <v>16</v>
       </c>
       <c r="C29" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="1">
+        <v>23</v>
+      </c>
+      <c r="B30" t="s">
         <v>30</v>
-      </c>
-      <c r="B30" s="1">
-        <v>23</v>
       </c>
       <c r="C30" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="1">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
         <v>37</v>
-      </c>
-      <c r="B31" s="1">
-        <v>6</v>
       </c>
       <c r="C31" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="1">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
         <v>39</v>
-      </c>
-      <c r="B32" s="1">
-        <v>10</v>
       </c>
       <c r="C32" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="1">
+        <v>24</v>
+      </c>
+      <c r="B33" t="s">
         <v>39</v>
-      </c>
-      <c r="B33" s="1">
-        <v>24</v>
       </c>
       <c r="C33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="1">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
         <v>42</v>
-      </c>
-      <c r="B34" s="1">
-        <v>1</v>
       </c>
       <c r="C34" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="1">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
         <v>42</v>
-      </c>
-      <c r="B35" s="1">
-        <v>1</v>
       </c>
       <c r="C35" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="1">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s">
         <v>42</v>
-      </c>
-      <c r="B36" s="1">
-        <v>8</v>
       </c>
       <c r="C36" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" s="1">
+        <v>22</v>
+      </c>
+      <c r="B37" t="s">
         <v>42</v>
-      </c>
-      <c r="B37" s="1">
-        <v>22</v>
       </c>
       <c r="C37" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" s="1">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
         <v>46</v>
-      </c>
-      <c r="B38" s="1">
-        <v>5</v>
       </c>
       <c r="C38" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" s="1">
+        <v>12</v>
+      </c>
+      <c r="B39" t="s">
         <v>46</v>
-      </c>
-      <c r="B39" s="1">
-        <v>12</v>
       </c>
       <c r="C39" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="1">
+        <v>19</v>
+      </c>
+      <c r="B40" t="s">
         <v>46</v>
-      </c>
-      <c r="B40" s="1">
-        <v>19</v>
       </c>
       <c r="C40" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" s="1">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
         <v>46</v>
-      </c>
-      <c r="B41" s="1">
-        <v>19</v>
       </c>
       <c r="C41" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="1">
+        <v>26</v>
+      </c>
+      <c r="B42" t="s">
         <v>46</v>
-      </c>
-      <c r="B42" s="1">
-        <v>26</v>
       </c>
       <c r="C42" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" t="s">
         <v>46</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="C43" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="1">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s">
         <v>53</v>
-      </c>
-      <c r="B44" s="1">
-        <v>3</v>
       </c>
       <c r="C44" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="A45" s="1">
+        <v>17</v>
+      </c>
+      <c r="B45" t="s">
         <v>53</v>
-      </c>
-      <c r="B45" s="1">
-        <v>17</v>
       </c>
       <c r="C45" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="A46" s="1">
+        <v>17</v>
+      </c>
+      <c r="B46" t="s">
         <v>53</v>
-      </c>
-      <c r="B46" s="1">
-        <v>17</v>
       </c>
       <c r="C46" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="A47" s="1">
+        <v>17</v>
+      </c>
+      <c r="B47" t="s">
         <v>53</v>
-      </c>
-      <c r="B47" s="1">
-        <v>17</v>
       </c>
       <c r="C47" t="s">
         <v>59</v>

</xml_diff>